<commit_message>
Adds P Medio, in between P and P1; removes typo
</commit_message>
<xml_diff>
--- a/BARCOLANA 2022 MARKS.xlsx
+++ b/BARCOLANA 2022 MARKS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Davide\FIV\GIVEMEFIVE\2022\BARCOLANA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F8DA0BF-1965-464E-B070-BE8DB6A89A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864FDBD8-AF62-4ED2-86DC-500307FF3C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{27A60614-E484-46BE-B74D-4FB6E6D643A6}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>P1</t>
   </si>
@@ -89,9 +89,6 @@
     <t>4</t>
   </si>
   <si>
-    <t>4 BIS</t>
-  </si>
-  <si>
     <t>45° 41,900’</t>
   </si>
   <si>
@@ -108,6 +105,12 @@
   </si>
   <si>
     <t>013° 45,400’</t>
+  </si>
+  <si>
+    <t>P MEDIO</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -115,7 +118,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -183,8 +186,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -500,18 +505,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B66EE71-1BF1-42E1-94C0-0A4259D48EA7}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="3" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -531,7 +536,7 @@
         <f>D1/60</f>
         <v>0.6748333333333334</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="4">
         <f>C1+E1</f>
         <v>45.674833333333332</v>
       </c>
@@ -548,7 +553,7 @@
         <f>I1/60</f>
         <v>0.74099999999999999</v>
       </c>
-      <c r="K1" s="3">
+      <c r="K1" s="4">
         <f>H1+J1</f>
         <v>13.741</v>
       </c>
@@ -567,11 +572,11 @@
         <v>41.255000000000003</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E9" si="0">D2/60</f>
+        <f t="shared" ref="E2:E10" si="0">D2/60</f>
         <v>0.68758333333333332</v>
       </c>
-      <c r="F2" s="3">
-        <f t="shared" ref="F2:F9" si="1">C2+E2</f>
+      <c r="F2" s="4">
+        <f t="shared" ref="F2:F10" si="1">C2+E2</f>
         <v>45.687583333333336</v>
       </c>
       <c r="G2" t="s">
@@ -584,283 +589,296 @@
         <v>41.91</v>
       </c>
       <c r="J2">
-        <f t="shared" ref="J2:J9" si="2">I2/60</f>
+        <f t="shared" ref="J2:J10" si="2">I2/60</f>
         <v>0.6984999999999999</v>
       </c>
-      <c r="K2" s="3">
-        <f t="shared" ref="K2:K9" si="3">H2+J2</f>
+      <c r="K2" s="4">
+        <f t="shared" ref="K2:K10" si="3">H2+J2</f>
         <v>13.698499999999999</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="4">
+        <f>AVERAGE(F1:F2)</f>
+        <v>45.681208333333331</v>
+      </c>
+      <c r="K3" s="4">
+        <f>AVERAGE(K1:K2)</f>
+        <v>13.719749999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>45</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>37.26</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <f t="shared" si="0"/>
         <v>0.621</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F4" s="4">
         <f t="shared" si="1"/>
         <v>45.621000000000002</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>11</v>
       </c>
-      <c r="H3">
-        <v>13</v>
-      </c>
-      <c r="I3">
+      <c r="H4">
+        <v>13</v>
+      </c>
+      <c r="I4">
         <v>40.25</v>
       </c>
-      <c r="J3">
+      <c r="J4">
         <f t="shared" si="2"/>
         <v>0.67083333333333328</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K4" s="4">
         <f t="shared" si="3"/>
         <v>13.670833333333333</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>45</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>38.134999999999998</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <f t="shared" si="0"/>
         <v>0.63558333333333328</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F5" s="4">
         <f t="shared" si="1"/>
         <v>45.635583333333336</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G5" t="s">
         <v>10</v>
       </c>
-      <c r="H4">
-        <v>13</v>
-      </c>
-      <c r="I4">
+      <c r="H5">
+        <v>13</v>
+      </c>
+      <c r="I5">
         <v>39.585999999999999</v>
       </c>
-      <c r="J4">
+      <c r="J5">
         <f t="shared" si="2"/>
         <v>0.65976666666666661</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K5" s="4">
         <f t="shared" si="3"/>
         <v>13.659766666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
         <v>45</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>38.033000000000001</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <f t="shared" si="0"/>
         <v>0.63388333333333335</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F6" s="4">
         <f t="shared" si="1"/>
         <v>45.63388333333333</v>
       </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5">
-        <v>13</v>
-      </c>
-      <c r="I5">
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6">
+        <v>13</v>
+      </c>
+      <c r="I6">
         <v>39.398000000000003</v>
       </c>
-      <c r="J5">
+      <c r="J6">
         <f t="shared" si="2"/>
         <v>0.6566333333333334</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K6" s="4">
         <f t="shared" si="3"/>
         <v>13.656633333333334</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6">
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7">
         <v>45</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>41.9</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <f t="shared" si="0"/>
         <v>0.69833333333333336</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F7" s="4">
         <f t="shared" si="1"/>
         <v>45.698333333333331</v>
       </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6">
-        <v>13</v>
-      </c>
-      <c r="I6">
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7">
+        <v>13</v>
+      </c>
+      <c r="I7">
         <v>41.9</v>
       </c>
-      <c r="J6">
+      <c r="J7">
         <f t="shared" si="2"/>
         <v>0.69833333333333336</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K7" s="4">
         <f t="shared" si="3"/>
         <v>13.698333333333334</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8">
         <v>45</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>41.98</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <f t="shared" si="0"/>
         <v>0.69966666666666666</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F8" s="4">
         <f t="shared" si="1"/>
         <v>45.699666666666666</v>
       </c>
-      <c r="G7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7">
-        <v>13</v>
-      </c>
-      <c r="I7">
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8">
+        <v>13</v>
+      </c>
+      <c r="I8">
         <v>41.61</v>
       </c>
-      <c r="J7">
+      <c r="J8">
         <f t="shared" si="2"/>
         <v>0.69350000000000001</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K8" s="4">
         <f t="shared" si="3"/>
         <v>13.6935</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>2</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>45</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>40.49</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <f t="shared" si="0"/>
         <v>0.6748333333333334</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F9" s="4">
         <f t="shared" si="1"/>
         <v>45.674833333333332</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G9" t="s">
         <v>3</v>
       </c>
-      <c r="H8">
-        <v>13</v>
-      </c>
-      <c r="I8">
+      <c r="H9">
+        <v>13</v>
+      </c>
+      <c r="I9">
         <v>44.46</v>
       </c>
-      <c r="J8">
+      <c r="J9">
         <f t="shared" si="2"/>
         <v>0.74099999999999999</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K9" s="4">
         <f t="shared" si="3"/>
         <v>13.741</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>45</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>39.200000000000003</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <f t="shared" si="0"/>
         <v>0.65333333333333343</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F10" s="4">
         <f t="shared" si="1"/>
         <v>45.653333333333336</v>
       </c>
-      <c r="G9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9">
-        <v>13</v>
-      </c>
-      <c r="I9">
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10">
+        <v>13</v>
+      </c>
+      <c r="I10">
         <v>45.4</v>
       </c>
-      <c r="J9">
+      <c r="J10">
         <f t="shared" si="2"/>
         <v>0.7566666666666666</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K10" s="4">
         <f t="shared" si="3"/>
         <v>13.756666666666666</v>
       </c>

</xml_diff>